<commit_message>
minor updates and removed PyCHAM_lite
PyCHAM_lite removed as main PyCHAM program can now act as lite when called programmatically
</commit_message>
<xml_diff>
--- a/PyCHAM/input/guaiacol/constraining_obs_wp.xlsx
+++ b/PyCHAM/input/guaiacol/constraining_obs_wp.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/PyCHAM/PyCHAM/input/guaiacol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CBDCD6-AA89-2641-82AE-313FC9B11058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3838FF83-94C1-184D-9BE4-2AFD6BF777A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12460" yWindow="8480" windowWidth="17480" windowHeight="13120" activeTab="1" xr2:uid="{7C74D523-2B60-6A4A-ACEB-A35EBE6838C7}"/>
+    <workbookView xWindow="18260" yWindow="6360" windowWidth="17480" windowHeight="13120" xr2:uid="{7C74D523-2B60-6A4A-ACEB-A35EBE6838C7}"/>
   </bookViews>
   <sheets>
     <sheet name="PyCHAMobs" sheetId="2" r:id="rId1"/>
     <sheet name="particle" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="J4_" localSheetId="0">PyCHAMobs!$H$2:$I$72</definedName>
+    <definedName name="J4_" localSheetId="0">PyCHAMobs!$H$2:$H$72</definedName>
     <definedName name="RH" localSheetId="0">PyCHAMobs!$F$2:$G$92</definedName>
     <definedName name="TEMP" localSheetId="0">PyCHAMobs!$A$2:$B$92</definedName>
   </definedNames>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Time (s)</t>
   </si>
@@ -107,15 +107,6 @@
   </si>
   <si>
     <t>HCHO</t>
-  </si>
-  <si>
-    <t>pconc_pm2.5</t>
-  </si>
-  <si>
-    <t>mean_rad_pm2.5</t>
-  </si>
-  <si>
-    <t>core_pm2.5_seedx</t>
   </si>
 </sst>
 </file>
@@ -489,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172C4B10-34B1-DA4C-872D-C5918B25BFA3}">
   <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,7 +491,7 @@
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
     <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -529,16 +520,16 @@
         <v>1</v>
       </c>
       <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
         <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -552,7 +543,7 @@
         <v>0.5</v>
       </c>
       <c r="D2">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -566,17 +557,17 @@
       <c r="H2" s="2">
         <v>436000000000</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2">
+        <v>1758465644</v>
+      </c>
+      <c r="J2" s="1">
+        <v>888000000000</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1050000000000</v>
+      </c>
+      <c r="L2" s="1">
         <v>10900000000000</v>
-      </c>
-      <c r="J2">
-        <v>1758465644</v>
-      </c>
-      <c r="K2" s="1">
-        <v>888000000000</v>
-      </c>
-      <c r="L2" s="1">
-        <v>1050000000000</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -590,7 +581,7 @@
         <v>0.4</v>
       </c>
       <c r="D3">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -605,16 +596,16 @@
         <v>562800000000</v>
       </c>
       <c r="I3">
+        <v>1758465644</v>
+      </c>
+      <c r="J3" s="1">
+        <v>906000000000</v>
+      </c>
+      <c r="K3" s="1">
+        <v>988000000000</v>
+      </c>
+      <c r="L3">
         <v>10574000000000</v>
-      </c>
-      <c r="J3">
-        <v>1758465644</v>
-      </c>
-      <c r="K3" s="1">
-        <v>906000000000</v>
-      </c>
-      <c r="L3" s="1">
-        <v>988000000000</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -628,7 +619,7 @@
         <v>0.3</v>
       </c>
       <c r="D4">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -643,16 +634,16 @@
         <v>689600000000</v>
       </c>
       <c r="I4">
+        <v>1758465644</v>
+      </c>
+      <c r="J4" s="1">
+        <v>930000000000</v>
+      </c>
+      <c r="K4" s="1">
+        <v>934000000000</v>
+      </c>
+      <c r="L4">
         <v>10248000000000</v>
-      </c>
-      <c r="J4">
-        <v>1758465644</v>
-      </c>
-      <c r="K4" s="1">
-        <v>930000000000</v>
-      </c>
-      <c r="L4" s="1">
-        <v>934000000000</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -666,7 +657,7 @@
         <v>0.3</v>
       </c>
       <c r="D5">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -681,16 +672,16 @@
         <v>816400000000</v>
       </c>
       <c r="I5">
+        <v>1758465644</v>
+      </c>
+      <c r="J5" s="1">
+        <v>892000000000</v>
+      </c>
+      <c r="K5" s="1">
+        <v>984000000000</v>
+      </c>
+      <c r="L5">
         <v>9922000000000</v>
-      </c>
-      <c r="J5">
-        <v>1758465644</v>
-      </c>
-      <c r="K5" s="1">
-        <v>892000000000</v>
-      </c>
-      <c r="L5" s="1">
-        <v>984000000000</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -704,7 +695,7 @@
         <v>0.3</v>
       </c>
       <c r="D6">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -719,16 +710,16 @@
         <v>943200000000</v>
       </c>
       <c r="I6">
+        <v>1758465644</v>
+      </c>
+      <c r="J6" s="1">
+        <v>831000000000</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1050000000000</v>
+      </c>
+      <c r="L6">
         <v>9596000000000</v>
-      </c>
-      <c r="J6">
-        <v>1758465644</v>
-      </c>
-      <c r="K6" s="1">
-        <v>831000000000</v>
-      </c>
-      <c r="L6" s="1">
-        <v>1050000000000</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -742,7 +733,7 @@
         <v>0.3</v>
       </c>
       <c r="D7">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -757,16 +748,16 @@
         <v>1070000000000</v>
       </c>
       <c r="I7">
+        <v>1758465644</v>
+      </c>
+      <c r="J7" s="1">
+        <v>754000000000</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1120000000000</v>
+      </c>
+      <c r="L7">
         <v>9270000000000</v>
-      </c>
-      <c r="J7">
-        <v>1758465644</v>
-      </c>
-      <c r="K7" s="1">
-        <v>754000000000</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1120000000000</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -780,7 +771,7 @@
         <v>0.3</v>
       </c>
       <c r="D8">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -795,16 +786,16 @@
         <v>1188000000000</v>
       </c>
       <c r="I8">
+        <v>9056967018</v>
+      </c>
+      <c r="J8" s="1">
+        <v>692000000000</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1180000000000</v>
+      </c>
+      <c r="L8">
         <v>9016000000000</v>
-      </c>
-      <c r="J8">
-        <v>9056967018</v>
-      </c>
-      <c r="K8" s="1">
-        <v>692000000000</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1180000000000</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -818,7 +809,7 @@
         <v>0.3</v>
       </c>
       <c r="D9">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -833,16 +824,16 @@
         <v>1306000000000</v>
       </c>
       <c r="I9">
+        <v>16167990656</v>
+      </c>
+      <c r="J9" s="1">
+        <v>651000000000</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1250000000000</v>
+      </c>
+      <c r="L9">
         <v>8762000000000</v>
-      </c>
-      <c r="J9">
-        <v>16167990656</v>
-      </c>
-      <c r="K9" s="1">
-        <v>651000000000</v>
-      </c>
-      <c r="L9" s="1">
-        <v>1250000000000</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -856,7 +847,7 @@
         <v>0.3</v>
       </c>
       <c r="D10">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -871,16 +862,16 @@
         <v>1424000000000</v>
       </c>
       <c r="I10">
+        <v>24617300084</v>
+      </c>
+      <c r="J10" s="1">
+        <v>609000000000</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1280000000000</v>
+      </c>
+      <c r="L10">
         <v>8508000000000</v>
-      </c>
-      <c r="J10">
-        <v>24617300084</v>
-      </c>
-      <c r="K10" s="1">
-        <v>609000000000</v>
-      </c>
-      <c r="L10" s="1">
-        <v>1280000000000</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -894,7 +885,7 @@
         <v>0.3</v>
       </c>
       <c r="D11">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -909,16 +900,16 @@
         <v>1542000000000</v>
       </c>
       <c r="I11">
+        <v>33123658774</v>
+      </c>
+      <c r="J11" s="1">
+        <v>555000000000</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1310000000000</v>
+      </c>
+      <c r="L11">
         <v>8254000000000</v>
-      </c>
-      <c r="J11">
-        <v>33123658774</v>
-      </c>
-      <c r="K11" s="1">
-        <v>555000000000</v>
-      </c>
-      <c r="L11" s="1">
-        <v>1310000000000</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -932,7 +923,7 @@
         <v>0.3</v>
       </c>
       <c r="D12">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -947,16 +938,16 @@
         <v>1660000000000</v>
       </c>
       <c r="I12">
+        <v>41499412781</v>
+      </c>
+      <c r="J12" s="1">
+        <v>518000000000</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1330000000000</v>
+      </c>
+      <c r="L12">
         <v>8000000000000</v>
-      </c>
-      <c r="J12">
-        <v>41499412781</v>
-      </c>
-      <c r="K12" s="1">
-        <v>518000000000</v>
-      </c>
-      <c r="L12" s="1">
-        <v>1330000000000</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -970,7 +961,7 @@
         <v>0.3</v>
       </c>
       <c r="D13">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -985,16 +976,16 @@
         <v>1756000000000</v>
       </c>
       <c r="I13">
+        <v>50468705728</v>
+      </c>
+      <c r="J13" s="1">
+        <v>504000000000</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1340000000000</v>
+      </c>
+      <c r="L13">
         <v>7774000000000</v>
-      </c>
-      <c r="J13">
-        <v>50468705728</v>
-      </c>
-      <c r="K13" s="1">
-        <v>504000000000</v>
-      </c>
-      <c r="L13" s="1">
-        <v>1340000000000</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1008,7 +999,7 @@
         <v>0.3</v>
       </c>
       <c r="D14">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1023,16 +1014,16 @@
         <v>1852000000000</v>
       </c>
       <c r="I14">
+        <v>60686968653</v>
+      </c>
+      <c r="J14" s="1">
+        <v>473000000000</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1350000000000</v>
+      </c>
+      <c r="L14">
         <v>7548000000000</v>
-      </c>
-      <c r="J14">
-        <v>60686968653</v>
-      </c>
-      <c r="K14" s="1">
-        <v>473000000000</v>
-      </c>
-      <c r="L14" s="1">
-        <v>1350000000000</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1046,7 +1037,7 @@
         <v>0.3</v>
       </c>
       <c r="D15">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1061,16 +1052,16 @@
         <v>1948000000000</v>
       </c>
       <c r="I15">
+        <v>70490484996</v>
+      </c>
+      <c r="J15" s="1">
+        <v>437000000000</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1340000000000</v>
+      </c>
+      <c r="L15">
         <v>7322000000000</v>
-      </c>
-      <c r="J15">
-        <v>70490484996</v>
-      </c>
-      <c r="K15" s="1">
-        <v>437000000000</v>
-      </c>
-      <c r="L15" s="1">
-        <v>1340000000000</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1084,7 +1075,7 @@
         <v>0.3</v>
       </c>
       <c r="D16">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1099,16 +1090,16 @@
         <v>2044000000000</v>
       </c>
       <c r="I16">
+        <v>79871811884</v>
+      </c>
+      <c r="J16" s="1">
+        <v>413000000000</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1350000000000</v>
+      </c>
+      <c r="L16">
         <v>7096000000000</v>
-      </c>
-      <c r="J16">
-        <v>79871811884</v>
-      </c>
-      <c r="K16" s="1">
-        <v>413000000000</v>
-      </c>
-      <c r="L16" s="1">
-        <v>1350000000000</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1122,7 +1113,7 @@
         <v>0.2</v>
       </c>
       <c r="D17">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1137,16 +1128,16 @@
         <v>2140000000000</v>
       </c>
       <c r="I17">
+        <v>91996741205</v>
+      </c>
+      <c r="J17" s="1">
+        <v>391000000000</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1340000000000</v>
+      </c>
+      <c r="L17">
         <v>6870000000000</v>
-      </c>
-      <c r="J17">
-        <v>91996741205</v>
-      </c>
-      <c r="K17" s="1">
-        <v>391000000000</v>
-      </c>
-      <c r="L17" s="1">
-        <v>1340000000000</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1160,7 +1151,7 @@
         <v>0.2</v>
       </c>
       <c r="D18">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1175,16 +1166,16 @@
         <v>2208000000000</v>
       </c>
       <c r="I18">
+        <v>102537000000</v>
+      </c>
+      <c r="J18" s="1">
+        <v>369000000000</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1340000000000</v>
+      </c>
+      <c r="L18">
         <v>6670000000000</v>
-      </c>
-      <c r="J18">
-        <v>102537000000</v>
-      </c>
-      <c r="K18" s="1">
-        <v>369000000000</v>
-      </c>
-      <c r="L18" s="1">
-        <v>1340000000000</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1198,7 +1189,7 @@
         <v>0.2</v>
       </c>
       <c r="D19">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1213,16 +1204,16 @@
         <v>2276000000000</v>
       </c>
       <c r="I19">
+        <v>112486000000</v>
+      </c>
+      <c r="J19" s="1">
+        <v>353000000000</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1320000000000</v>
+      </c>
+      <c r="L19">
         <v>6470000000000</v>
-      </c>
-      <c r="J19">
-        <v>112486000000</v>
-      </c>
-      <c r="K19" s="1">
-        <v>353000000000</v>
-      </c>
-      <c r="L19" s="1">
-        <v>1320000000000</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1236,7 +1227,7 @@
         <v>0.2</v>
       </c>
       <c r="D20">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1251,16 +1242,16 @@
         <v>2344000000000</v>
       </c>
       <c r="I20">
+        <v>126114000000</v>
+      </c>
+      <c r="J20" s="1">
+        <v>349000000000</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1310000000000</v>
+      </c>
+      <c r="L20">
         <v>6270000000000</v>
-      </c>
-      <c r="J20">
-        <v>126114000000</v>
-      </c>
-      <c r="K20" s="1">
-        <v>349000000000</v>
-      </c>
-      <c r="L20" s="1">
-        <v>1310000000000</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1274,7 +1265,7 @@
         <v>0.2</v>
       </c>
       <c r="D21">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1289,16 +1280,16 @@
         <v>2412000000000</v>
       </c>
       <c r="I21">
+        <v>146740000000</v>
+      </c>
+      <c r="J21" s="1">
+        <v>348000000000</v>
+      </c>
+      <c r="K21" s="1">
+        <v>1300000000000</v>
+      </c>
+      <c r="L21">
         <v>6070000000000</v>
-      </c>
-      <c r="J21">
-        <v>146740000000</v>
-      </c>
-      <c r="K21" s="1">
-        <v>348000000000</v>
-      </c>
-      <c r="L21" s="1">
-        <v>1300000000000</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -1312,7 +1303,7 @@
         <v>0.2</v>
       </c>
       <c r="D22">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1327,16 +1318,16 @@
         <v>2480000000000</v>
       </c>
       <c r="I22">
+        <v>158982000000</v>
+      </c>
+      <c r="J22" s="1">
+        <v>344000000000</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1290000000000</v>
+      </c>
+      <c r="L22">
         <v>5870000000000</v>
-      </c>
-      <c r="J22">
-        <v>158982000000</v>
-      </c>
-      <c r="K22" s="1">
-        <v>344000000000</v>
-      </c>
-      <c r="L22" s="1">
-        <v>1290000000000</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -1350,7 +1341,7 @@
         <v>0.2</v>
       </c>
       <c r="D23">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1365,16 +1356,16 @@
         <v>2544000000000</v>
       </c>
       <c r="I23">
+        <v>165527000000</v>
+      </c>
+      <c r="J23" s="1">
+        <v>339000000000</v>
+      </c>
+      <c r="K23" s="1">
+        <v>1270000000000</v>
+      </c>
+      <c r="L23">
         <v>5696000000000</v>
-      </c>
-      <c r="J23">
-        <v>165527000000</v>
-      </c>
-      <c r="K23" s="1">
-        <v>339000000000</v>
-      </c>
-      <c r="L23" s="1">
-        <v>1270000000000</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -1388,7 +1379,7 @@
         <v>0.2</v>
       </c>
       <c r="D24">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1403,16 +1394,16 @@
         <v>2608000000000</v>
       </c>
       <c r="I24">
+        <v>188466000000</v>
+      </c>
+      <c r="J24" s="1">
+        <v>329000000000</v>
+      </c>
+      <c r="K24" s="1">
+        <v>1250000000000</v>
+      </c>
+      <c r="L24">
         <v>5522000000000</v>
-      </c>
-      <c r="J24">
-        <v>188466000000</v>
-      </c>
-      <c r="K24" s="1">
-        <v>329000000000</v>
-      </c>
-      <c r="L24" s="1">
-        <v>1250000000000</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -1426,7 +1417,7 @@
         <v>0.2</v>
       </c>
       <c r="D25">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1441,16 +1432,16 @@
         <v>2672000000000</v>
       </c>
       <c r="I25">
+        <v>201501000000</v>
+      </c>
+      <c r="J25" s="1">
+        <v>318000000000</v>
+      </c>
+      <c r="K25" s="1">
+        <v>1230000000000</v>
+      </c>
+      <c r="L25">
         <v>5348000000000</v>
-      </c>
-      <c r="J25">
-        <v>201501000000</v>
-      </c>
-      <c r="K25" s="1">
-        <v>318000000000</v>
-      </c>
-      <c r="L25" s="1">
-        <v>1230000000000</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -1464,7 +1455,7 @@
         <v>0.2</v>
       </c>
       <c r="D26">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1479,16 +1470,16 @@
         <v>2736000000000</v>
       </c>
       <c r="I26">
+        <v>206117000000</v>
+      </c>
+      <c r="J26" s="1">
+        <v>308000000000</v>
+      </c>
+      <c r="K26" s="1">
+        <v>1220000000000</v>
+      </c>
+      <c r="L26">
         <v>5174000000000</v>
-      </c>
-      <c r="J26">
-        <v>206117000000</v>
-      </c>
-      <c r="K26" s="1">
-        <v>308000000000</v>
-      </c>
-      <c r="L26" s="1">
-        <v>1220000000000</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -1502,7 +1493,7 @@
         <v>0.2</v>
       </c>
       <c r="D27">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1517,16 +1508,16 @@
         <v>2800000000000</v>
       </c>
       <c r="I27">
+        <v>213442000000</v>
+      </c>
+      <c r="J27" s="1">
+        <v>295000000000</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1220000000000</v>
+      </c>
+      <c r="L27">
         <v>5000000000000</v>
-      </c>
-      <c r="J27">
-        <v>213442000000</v>
-      </c>
-      <c r="K27" s="1">
-        <v>295000000000</v>
-      </c>
-      <c r="L27" s="1">
-        <v>1220000000000</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -1540,7 +1531,7 @@
         <v>0.2</v>
       </c>
       <c r="D28">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1555,16 +1546,16 @@
         <v>2850000000000</v>
       </c>
       <c r="I28">
+        <v>220717000000</v>
+      </c>
+      <c r="J28" s="1">
+        <v>281000000000</v>
+      </c>
+      <c r="K28" s="1">
+        <v>1210000000000</v>
+      </c>
+      <c r="L28">
         <v>4872000000000</v>
-      </c>
-      <c r="J28">
-        <v>220717000000</v>
-      </c>
-      <c r="K28" s="1">
-        <v>281000000000</v>
-      </c>
-      <c r="L28" s="1">
-        <v>1210000000000</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -1578,7 +1569,7 @@
         <v>0.2</v>
       </c>
       <c r="D29">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -1593,16 +1584,16 @@
         <v>2900000000000</v>
       </c>
       <c r="I29">
+        <v>228777000000</v>
+      </c>
+      <c r="J29" s="1">
+        <v>270000000000</v>
+      </c>
+      <c r="K29" s="1">
+        <v>1170000000000</v>
+      </c>
+      <c r="L29">
         <v>4744000000000</v>
-      </c>
-      <c r="J29">
-        <v>228777000000</v>
-      </c>
-      <c r="K29" s="1">
-        <v>270000000000</v>
-      </c>
-      <c r="L29" s="1">
-        <v>1170000000000</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -1616,7 +1607,7 @@
         <v>0.2</v>
       </c>
       <c r="D30">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1631,16 +1622,16 @@
         <v>2950000000000</v>
       </c>
       <c r="I30">
+        <v>237628000000</v>
+      </c>
+      <c r="J30" s="1">
+        <v>260000000000</v>
+      </c>
+      <c r="K30" s="1">
+        <v>1150000000000</v>
+      </c>
+      <c r="L30">
         <v>4616000000000</v>
-      </c>
-      <c r="J30">
-        <v>237628000000</v>
-      </c>
-      <c r="K30" s="1">
-        <v>260000000000</v>
-      </c>
-      <c r="L30" s="1">
-        <v>1150000000000</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -1654,7 +1645,7 @@
         <v>0.2</v>
       </c>
       <c r="D31">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1669,16 +1660,16 @@
         <v>3000000000000</v>
       </c>
       <c r="I31">
+        <v>255626000000</v>
+      </c>
+      <c r="J31" s="1">
+        <v>246000000000</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1130000000000</v>
+      </c>
+      <c r="L31">
         <v>4488000000000</v>
-      </c>
-      <c r="J31">
-        <v>255626000000</v>
-      </c>
-      <c r="K31" s="1">
-        <v>246000000000</v>
-      </c>
-      <c r="L31" s="1">
-        <v>1130000000000</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -1692,7 +1683,7 @@
         <v>0.2</v>
       </c>
       <c r="D32">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1707,16 +1698,16 @@
         <v>3050000000000</v>
       </c>
       <c r="I32">
+        <v>258358000000</v>
+      </c>
+      <c r="J32" s="1">
+        <v>238000000000</v>
+      </c>
+      <c r="K32" s="1">
+        <v>1110000000000</v>
+      </c>
+      <c r="L32">
         <v>4360000000000</v>
-      </c>
-      <c r="J32">
-        <v>258358000000</v>
-      </c>
-      <c r="K32" s="1">
-        <v>238000000000</v>
-      </c>
-      <c r="L32" s="1">
-        <v>1110000000000</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -1730,7 +1721,7 @@
         <v>0.2</v>
       </c>
       <c r="D33">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1745,16 +1736,16 @@
         <v>3096000000000</v>
       </c>
       <c r="I33">
+        <v>259209000000</v>
+      </c>
+      <c r="J33" s="1">
+        <v>230000000000</v>
+      </c>
+      <c r="K33" s="1">
+        <v>1090000000000</v>
+      </c>
+      <c r="L33">
         <v>4256000000000</v>
-      </c>
-      <c r="J33">
-        <v>259209000000</v>
-      </c>
-      <c r="K33" s="1">
-        <v>230000000000</v>
-      </c>
-      <c r="L33" s="1">
-        <v>1090000000000</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -1768,7 +1759,7 @@
         <v>0.2</v>
       </c>
       <c r="D34">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1783,16 +1774,16 @@
         <v>3142000000000</v>
       </c>
       <c r="I34">
+        <v>261623000000</v>
+      </c>
+      <c r="J34" s="1">
+        <v>220000000000</v>
+      </c>
+      <c r="K34" s="1">
+        <v>1070000000000</v>
+      </c>
+      <c r="L34">
         <v>4152000000000</v>
-      </c>
-      <c r="J34">
-        <v>261623000000</v>
-      </c>
-      <c r="K34" s="1">
-        <v>220000000000</v>
-      </c>
-      <c r="L34" s="1">
-        <v>1070000000000</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -1806,7 +1797,7 @@
         <v>0.2</v>
       </c>
       <c r="D35">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1821,16 +1812,16 @@
         <v>3188000000000</v>
       </c>
       <c r="I35">
+        <v>268158000000</v>
+      </c>
+      <c r="J35" s="1">
+        <v>215000000000</v>
+      </c>
+      <c r="K35" s="1">
+        <v>1050000000000</v>
+      </c>
+      <c r="L35">
         <v>4048000000000</v>
-      </c>
-      <c r="J35">
-        <v>268158000000</v>
-      </c>
-      <c r="K35" s="1">
-        <v>215000000000</v>
-      </c>
-      <c r="L35" s="1">
-        <v>1050000000000</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
@@ -1844,7 +1835,7 @@
         <v>0.2</v>
       </c>
       <c r="D36">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1859,16 +1850,16 @@
         <v>3234000000000</v>
       </c>
       <c r="I36">
+        <v>282585000000</v>
+      </c>
+      <c r="J36" s="1">
+        <v>208000000000</v>
+      </c>
+      <c r="K36" s="1">
+        <v>1030000000000</v>
+      </c>
+      <c r="L36">
         <v>3944000000000</v>
-      </c>
-      <c r="J36">
-        <v>282585000000</v>
-      </c>
-      <c r="K36" s="1">
-        <v>208000000000</v>
-      </c>
-      <c r="L36" s="1">
-        <v>1030000000000</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
@@ -1882,7 +1873,7 @@
         <v>0.2</v>
       </c>
       <c r="D37">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1897,16 +1888,16 @@
         <v>3280000000000</v>
       </c>
       <c r="I37">
+        <v>298319000000</v>
+      </c>
+      <c r="J37" s="1">
+        <v>201000000000</v>
+      </c>
+      <c r="K37" s="1">
+        <v>1010000000000</v>
+      </c>
+      <c r="L37">
         <v>3840000000000</v>
-      </c>
-      <c r="J37">
-        <v>298319000000</v>
-      </c>
-      <c r="K37" s="1">
-        <v>201000000000</v>
-      </c>
-      <c r="L37" s="1">
-        <v>1010000000000</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -1920,7 +1911,7 @@
         <v>0.2</v>
       </c>
       <c r="D38">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1935,16 +1926,16 @@
         <v>3318000000000</v>
       </c>
       <c r="I38">
+        <v>301686000000</v>
+      </c>
+      <c r="J38" s="1">
+        <v>194000000000</v>
+      </c>
+      <c r="K38" s="1">
+        <v>991000000000</v>
+      </c>
+      <c r="L38">
         <v>3750000000000</v>
-      </c>
-      <c r="J38">
-        <v>301686000000</v>
-      </c>
-      <c r="K38" s="1">
-        <v>194000000000</v>
-      </c>
-      <c r="L38" s="1">
-        <v>991000000000</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -1958,7 +1949,7 @@
         <v>0.2</v>
       </c>
       <c r="D39">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -1973,16 +1964,16 @@
         <v>3356000000000</v>
       </c>
       <c r="I39">
+        <v>303747000000</v>
+      </c>
+      <c r="J39" s="1">
+        <v>186000000000</v>
+      </c>
+      <c r="K39" s="1">
+        <v>960000000000</v>
+      </c>
+      <c r="L39">
         <v>3660000000000</v>
-      </c>
-      <c r="J39">
-        <v>303747000000</v>
-      </c>
-      <c r="K39" s="1">
-        <v>186000000000</v>
-      </c>
-      <c r="L39" s="1">
-        <v>960000000000</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
@@ -1996,7 +1987,7 @@
         <v>0.2</v>
       </c>
       <c r="D40">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -2011,16 +2002,16 @@
         <v>3432000000000</v>
       </c>
       <c r="I40">
+        <v>326838000000</v>
+      </c>
+      <c r="J40" s="1">
+        <v>173000000000</v>
+      </c>
+      <c r="K40" s="1">
+        <v>934000000000</v>
+      </c>
+      <c r="L40">
         <v>3480000000000</v>
-      </c>
-      <c r="J40">
-        <v>326838000000</v>
-      </c>
-      <c r="K40" s="1">
-        <v>173000000000</v>
-      </c>
-      <c r="L40" s="1">
-        <v>934000000000</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -2034,7 +2025,7 @@
         <v>0.2</v>
       </c>
       <c r="D41">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -2049,16 +2040,16 @@
         <v>3470000000000</v>
       </c>
       <c r="I41">
+        <v>370110000000</v>
+      </c>
+      <c r="J41" s="1">
+        <v>167000000000</v>
+      </c>
+      <c r="K41" s="1">
+        <v>917000000000</v>
+      </c>
+      <c r="L41">
         <v>3390000000000</v>
-      </c>
-      <c r="J41">
-        <v>370110000000</v>
-      </c>
-      <c r="K41" s="1">
-        <v>167000000000</v>
-      </c>
-      <c r="L41" s="1">
-        <v>917000000000</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
@@ -2072,7 +2063,7 @@
         <v>0.2</v>
       </c>
       <c r="D42">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -2087,16 +2078,16 @@
         <v>3502000000000</v>
       </c>
       <c r="I42">
+        <v>383311000000</v>
+      </c>
+      <c r="J42" s="1">
+        <v>159000000000</v>
+      </c>
+      <c r="K42" s="1">
+        <v>899000000000</v>
+      </c>
+      <c r="L42">
         <v>3314000000000</v>
-      </c>
-      <c r="J42">
-        <v>383311000000</v>
-      </c>
-      <c r="K42" s="1">
-        <v>159000000000</v>
-      </c>
-      <c r="L42" s="1">
-        <v>899000000000</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -2110,7 +2101,7 @@
         <v>0.2</v>
       </c>
       <c r="D43">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -2125,16 +2116,16 @@
         <v>3534000000000</v>
       </c>
       <c r="I43">
+        <v>369750000000</v>
+      </c>
+      <c r="J43" s="1">
+        <v>155000000000</v>
+      </c>
+      <c r="K43" s="1">
+        <v>880000000000</v>
+      </c>
+      <c r="L43">
         <v>3238000000000</v>
-      </c>
-      <c r="J43">
-        <v>369750000000</v>
-      </c>
-      <c r="K43" s="1">
-        <v>155000000000</v>
-      </c>
-      <c r="L43" s="1">
-        <v>880000000000</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -2148,7 +2139,7 @@
         <v>0.2</v>
       </c>
       <c r="D44">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -2163,16 +2154,16 @@
         <v>3566000000000</v>
       </c>
       <c r="I44">
+        <v>364267000000</v>
+      </c>
+      <c r="J44" s="1">
+        <v>148000000000</v>
+      </c>
+      <c r="K44" s="1">
+        <v>863000000000</v>
+      </c>
+      <c r="L44">
         <v>3162000000000</v>
-      </c>
-      <c r="J44">
-        <v>364267000000</v>
-      </c>
-      <c r="K44" s="1">
-        <v>148000000000</v>
-      </c>
-      <c r="L44" s="1">
-        <v>863000000000</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
@@ -2186,7 +2177,7 @@
         <v>0.2</v>
       </c>
       <c r="D45">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -2201,16 +2192,16 @@
         <v>3598000000000</v>
       </c>
       <c r="I45">
+        <v>363907000000</v>
+      </c>
+      <c r="J45" s="1">
+        <v>143000000000</v>
+      </c>
+      <c r="K45" s="1">
+        <v>846000000000</v>
+      </c>
+      <c r="L45">
         <v>3086000000000</v>
-      </c>
-      <c r="J45">
-        <v>363907000000</v>
-      </c>
-      <c r="K45" s="1">
-        <v>143000000000</v>
-      </c>
-      <c r="L45" s="1">
-        <v>846000000000</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
@@ -2224,7 +2215,7 @@
         <v>0.2</v>
       </c>
       <c r="D46">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -2239,16 +2230,16 @@
         <v>3630000000000</v>
       </c>
       <c r="I46">
+        <v>369246000000</v>
+      </c>
+      <c r="J46" s="1">
+        <v>138000000000</v>
+      </c>
+      <c r="K46" s="1">
+        <v>826000000000</v>
+      </c>
+      <c r="L46">
         <v>3010000000000</v>
-      </c>
-      <c r="J46">
-        <v>369246000000</v>
-      </c>
-      <c r="K46" s="1">
-        <v>138000000000</v>
-      </c>
-      <c r="L46" s="1">
-        <v>826000000000</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -2262,7 +2253,7 @@
         <v>0.2</v>
       </c>
       <c r="D47">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -2277,16 +2268,16 @@
         <v>3651666666666.6602</v>
       </c>
       <c r="I47">
+        <v>387357000000</v>
+      </c>
+      <c r="J47" s="1">
+        <v>137000000000</v>
+      </c>
+      <c r="K47" s="1">
+        <v>809000000000</v>
+      </c>
+      <c r="L47">
         <v>2956666666666.6602</v>
-      </c>
-      <c r="J47">
-        <v>387357000000</v>
-      </c>
-      <c r="K47" s="1">
-        <v>137000000000</v>
-      </c>
-      <c r="L47" s="1">
-        <v>809000000000</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -2300,7 +2291,7 @@
         <v>0.2</v>
       </c>
       <c r="D48">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -2315,16 +2306,16 @@
         <v>3673333333333.3301</v>
       </c>
       <c r="I48">
+        <v>401610000000</v>
+      </c>
+      <c r="J48" s="1">
+        <v>132000000000</v>
+      </c>
+      <c r="K48" s="1">
+        <v>792000000000</v>
+      </c>
+      <c r="L48">
         <v>2903333333333.3301</v>
-      </c>
-      <c r="J48">
-        <v>401610000000</v>
-      </c>
-      <c r="K48" s="1">
-        <v>132000000000</v>
-      </c>
-      <c r="L48" s="1">
-        <v>792000000000</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -2338,7 +2329,7 @@
         <v>0.2</v>
       </c>
       <c r="D49">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -2353,16 +2344,16 @@
         <v>3695000000000</v>
       </c>
       <c r="I49">
+        <v>406518000000</v>
+      </c>
+      <c r="J49" s="1">
+        <v>130000000000</v>
+      </c>
+      <c r="K49" s="1">
+        <v>766000000000</v>
+      </c>
+      <c r="L49">
         <v>2850000000000</v>
-      </c>
-      <c r="J49">
-        <v>406518000000</v>
-      </c>
-      <c r="K49" s="1">
-        <v>130000000000</v>
-      </c>
-      <c r="L49" s="1">
-        <v>766000000000</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
@@ -2376,7 +2367,7 @@
         <v>0.2</v>
       </c>
       <c r="D50">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -2391,16 +2382,16 @@
         <v>3716666666666.6602</v>
       </c>
       <c r="I50">
+        <v>404686000000</v>
+      </c>
+      <c r="J50" s="1">
+        <v>124000000000</v>
+      </c>
+      <c r="K50" s="1">
+        <v>754000000000</v>
+      </c>
+      <c r="L50">
         <v>2796666666666.6602</v>
-      </c>
-      <c r="J50">
-        <v>404686000000</v>
-      </c>
-      <c r="K50" s="1">
-        <v>124000000000</v>
-      </c>
-      <c r="L50" s="1">
-        <v>754000000000</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -2414,7 +2405,7 @@
         <v>0.2</v>
       </c>
       <c r="D51">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -2429,16 +2420,16 @@
         <v>3738333333333.3301</v>
       </c>
       <c r="I51">
+        <v>419110000000</v>
+      </c>
+      <c r="J51" s="1">
+        <v>122000000000</v>
+      </c>
+      <c r="K51" s="1">
+        <v>742000000000</v>
+      </c>
+      <c r="L51">
         <v>2743333333333.3301</v>
-      </c>
-      <c r="J51">
-        <v>419110000000</v>
-      </c>
-      <c r="K51" s="1">
-        <v>122000000000</v>
-      </c>
-      <c r="L51" s="1">
-        <v>742000000000</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -2452,7 +2443,7 @@
         <v>0.2</v>
       </c>
       <c r="D52">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -2467,16 +2458,16 @@
         <v>3760000000000</v>
       </c>
       <c r="I52">
+        <v>429770000000</v>
+      </c>
+      <c r="J52" s="1">
+        <v>119000000000</v>
+      </c>
+      <c r="K52" s="1">
+        <v>732000000000</v>
+      </c>
+      <c r="L52">
         <v>2690000000000</v>
-      </c>
-      <c r="J52">
-        <v>429770000000</v>
-      </c>
-      <c r="K52" s="1">
-        <v>119000000000</v>
-      </c>
-      <c r="L52" s="1">
-        <v>732000000000</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
@@ -2490,7 +2481,7 @@
         <v>0.2</v>
       </c>
       <c r="D53">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -2505,16 +2496,16 @@
         <v>3782000000000</v>
       </c>
       <c r="I53">
+        <v>468560000000</v>
+      </c>
+      <c r="J53" s="1">
+        <v>117000000000</v>
+      </c>
+      <c r="K53" s="1">
+        <v>715000000000</v>
+      </c>
+      <c r="L53">
         <v>2640000000000</v>
-      </c>
-      <c r="J53">
-        <v>468560000000</v>
-      </c>
-      <c r="K53" s="1">
-        <v>117000000000</v>
-      </c>
-      <c r="L53" s="1">
-        <v>715000000000</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
@@ -2528,7 +2519,7 @@
         <v>0.2</v>
       </c>
       <c r="D54">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -2543,16 +2534,16 @@
         <v>3804000000000</v>
       </c>
       <c r="I54">
+        <v>469350000000</v>
+      </c>
+      <c r="J54" s="1">
+        <v>113000000000</v>
+      </c>
+      <c r="K54" s="1">
+        <v>701000000000</v>
+      </c>
+      <c r="L54">
         <v>2590000000000</v>
-      </c>
-      <c r="J54">
-        <v>469350000000</v>
-      </c>
-      <c r="K54" s="1">
-        <v>113000000000</v>
-      </c>
-      <c r="L54" s="1">
-        <v>701000000000</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -2566,7 +2557,7 @@
         <v>0.2</v>
       </c>
       <c r="D55">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -2581,16 +2572,16 @@
         <v>3826000000000</v>
       </c>
       <c r="I55">
+        <v>456237000000</v>
+      </c>
+      <c r="J55" s="1">
+        <v>111000000000</v>
+      </c>
+      <c r="K55" s="1">
+        <v>684000000000</v>
+      </c>
+      <c r="L55">
         <v>2540000000000</v>
-      </c>
-      <c r="J55">
-        <v>456237000000</v>
-      </c>
-      <c r="K55" s="1">
-        <v>111000000000</v>
-      </c>
-      <c r="L55" s="1">
-        <v>684000000000</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -2604,7 +2595,7 @@
         <v>0.2</v>
       </c>
       <c r="D56">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -2619,16 +2610,16 @@
         <v>3848000000000</v>
       </c>
       <c r="I56">
+        <v>437304000000</v>
+      </c>
+      <c r="J56" s="1">
+        <v>105000000000</v>
+      </c>
+      <c r="K56" s="1">
+        <v>673000000000</v>
+      </c>
+      <c r="L56">
         <v>2490000000000</v>
-      </c>
-      <c r="J56">
-        <v>437304000000</v>
-      </c>
-      <c r="K56" s="1">
-        <v>105000000000</v>
-      </c>
-      <c r="L56" s="1">
-        <v>673000000000</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
@@ -2642,7 +2633,7 @@
         <v>0.2</v>
       </c>
       <c r="D57">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -2657,16 +2648,16 @@
         <v>3870000000000</v>
       </c>
       <c r="I57">
+        <v>429154000000</v>
+      </c>
+      <c r="J57" s="1">
+        <v>102000000000</v>
+      </c>
+      <c r="K57" s="1">
+        <v>667000000000</v>
+      </c>
+      <c r="L57">
         <v>2440000000000</v>
-      </c>
-      <c r="J57">
-        <v>429154000000</v>
-      </c>
-      <c r="K57" s="1">
-        <v>102000000000</v>
-      </c>
-      <c r="L57" s="1">
-        <v>667000000000</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -2680,7 +2671,7 @@
         <v>0.2</v>
       </c>
       <c r="D58">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -2695,16 +2686,16 @@
         <v>3892000000000</v>
       </c>
       <c r="I58">
+        <v>460321000000</v>
+      </c>
+      <c r="J58" s="1">
+        <v>99900000000</v>
+      </c>
+      <c r="K58" s="1">
+        <v>667000000000</v>
+      </c>
+      <c r="L58">
         <v>2396000000000</v>
-      </c>
-      <c r="J58">
-        <v>460321000000</v>
-      </c>
-      <c r="K58" s="1">
-        <v>99900000000</v>
-      </c>
-      <c r="L58" s="1">
-        <v>667000000000</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
@@ -2718,7 +2709,7 @@
         <v>0.2</v>
       </c>
       <c r="D59">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -2733,16 +2724,16 @@
         <v>3914000000000</v>
       </c>
       <c r="I59">
+        <v>477961000000</v>
+      </c>
+      <c r="J59" s="1">
+        <v>98200000000</v>
+      </c>
+      <c r="K59" s="1">
+        <v>637000000000</v>
+      </c>
+      <c r="L59">
         <v>2352000000000</v>
-      </c>
-      <c r="J59">
-        <v>477961000000</v>
-      </c>
-      <c r="K59" s="1">
-        <v>98200000000</v>
-      </c>
-      <c r="L59" s="1">
-        <v>637000000000</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
@@ -2756,7 +2747,7 @@
         <v>0.2</v>
       </c>
       <c r="D60">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -2771,16 +2762,16 @@
         <v>3936000000000</v>
       </c>
       <c r="I60">
+        <v>483417000000</v>
+      </c>
+      <c r="J60" s="1">
+        <v>96200000000</v>
+      </c>
+      <c r="K60" s="1">
+        <v>618000000000</v>
+      </c>
+      <c r="L60">
         <v>2308000000000</v>
-      </c>
-      <c r="J60">
-        <v>483417000000</v>
-      </c>
-      <c r="K60" s="1">
-        <v>96200000000</v>
-      </c>
-      <c r="L60" s="1">
-        <v>618000000000</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
@@ -2794,7 +2785,7 @@
         <v>0.2</v>
       </c>
       <c r="D61">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -2809,16 +2800,16 @@
         <v>3958000000000</v>
       </c>
       <c r="I61">
+        <v>474513000000</v>
+      </c>
+      <c r="J61" s="1">
+        <v>93500000000</v>
+      </c>
+      <c r="K61" s="1">
+        <v>603000000000</v>
+      </c>
+      <c r="L61">
         <v>2264000000000</v>
-      </c>
-      <c r="J61">
-        <v>474513000000</v>
-      </c>
-      <c r="K61" s="1">
-        <v>93500000000</v>
-      </c>
-      <c r="L61" s="1">
-        <v>603000000000</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
@@ -2832,7 +2823,7 @@
         <v>0.2</v>
       </c>
       <c r="D62">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -2847,16 +2838,16 @@
         <v>3980000000000</v>
       </c>
       <c r="I62">
+        <v>456301000000</v>
+      </c>
+      <c r="J62" s="1">
+        <v>91500000000</v>
+      </c>
+      <c r="K62" s="1">
+        <v>580000000000</v>
+      </c>
+      <c r="L62">
         <v>2220000000000</v>
-      </c>
-      <c r="J62">
-        <v>456301000000</v>
-      </c>
-      <c r="K62" s="1">
-        <v>91500000000</v>
-      </c>
-      <c r="L62" s="1">
-        <v>580000000000</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
@@ -2870,7 +2861,7 @@
         <v>0.2</v>
       </c>
       <c r="D63">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -2885,16 +2876,16 @@
         <v>3994000000000</v>
       </c>
       <c r="I63">
+        <v>453540000000</v>
+      </c>
+      <c r="J63" s="1">
+        <v>87300000000</v>
+      </c>
+      <c r="K63" s="1">
+        <v>569000000000</v>
+      </c>
+      <c r="L63">
         <v>2176000000000</v>
-      </c>
-      <c r="J63">
-        <v>453540000000</v>
-      </c>
-      <c r="K63" s="1">
-        <v>87300000000</v>
-      </c>
-      <c r="L63" s="1">
-        <v>569000000000</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
@@ -2908,7 +2899,7 @@
         <v>0.2</v>
       </c>
       <c r="D64">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -2923,16 +2914,16 @@
         <v>4008000000000</v>
       </c>
       <c r="I64">
+        <v>674240000000</v>
+      </c>
+      <c r="J64" s="1">
+        <v>85100000000</v>
+      </c>
+      <c r="K64" s="1">
+        <v>561000000000</v>
+      </c>
+      <c r="L64">
         <v>2132000000000</v>
-      </c>
-      <c r="J64">
-        <v>674240000000</v>
-      </c>
-      <c r="K64" s="1">
-        <v>85100000000</v>
-      </c>
-      <c r="L64" s="1">
-        <v>561000000000</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
@@ -2946,7 +2937,7 @@
         <v>0.2</v>
       </c>
       <c r="D65">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -2961,16 +2952,16 @@
         <v>4022000000000</v>
       </c>
       <c r="I65">
+        <v>808212000000</v>
+      </c>
+      <c r="J65" s="1">
+        <v>85100000000</v>
+      </c>
+      <c r="K65" s="1">
+        <v>550000000000</v>
+      </c>
+      <c r="L65">
         <v>2088000000000</v>
-      </c>
-      <c r="J65">
-        <v>808212000000</v>
-      </c>
-      <c r="K65" s="1">
-        <v>85100000000</v>
-      </c>
-      <c r="L65" s="1">
-        <v>550000000000</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
@@ -2984,7 +2975,7 @@
         <v>0.2</v>
       </c>
       <c r="D66">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -2999,16 +2990,16 @@
         <v>4036000000000</v>
       </c>
       <c r="I66">
+        <v>653666000000</v>
+      </c>
+      <c r="J66" s="1">
+        <v>83600000000</v>
+      </c>
+      <c r="K66" s="1">
+        <v>540000000000</v>
+      </c>
+      <c r="L66">
         <v>2044000000000</v>
-      </c>
-      <c r="J66">
-        <v>653666000000</v>
-      </c>
-      <c r="K66" s="1">
-        <v>83600000000</v>
-      </c>
-      <c r="L66" s="1">
-        <v>540000000000</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
@@ -3022,7 +3013,7 @@
         <v>0.2</v>
       </c>
       <c r="D67">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -3037,16 +3028,16 @@
         <v>4050000000000</v>
       </c>
       <c r="I67">
+        <v>547203000000</v>
+      </c>
+      <c r="J67" s="1">
+        <v>80200000000</v>
+      </c>
+      <c r="K67" s="1">
+        <v>528000000000</v>
+      </c>
+      <c r="L67">
         <v>2000000000000</v>
-      </c>
-      <c r="J67">
-        <v>547203000000</v>
-      </c>
-      <c r="K67" s="1">
-        <v>80200000000</v>
-      </c>
-      <c r="L67" s="1">
-        <v>528000000000</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
@@ -3060,7 +3051,7 @@
         <v>0.2</v>
       </c>
       <c r="D68">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -3075,16 +3066,16 @@
         <v>4064000000000</v>
       </c>
       <c r="I68">
+        <v>572195000000</v>
+      </c>
+      <c r="J68" s="1">
+        <v>77000000000</v>
+      </c>
+      <c r="K68" s="1">
+        <v>518000000000</v>
+      </c>
+      <c r="L68">
         <v>1972000000000</v>
-      </c>
-      <c r="J68">
-        <v>572195000000</v>
-      </c>
-      <c r="K68" s="1">
-        <v>77000000000</v>
-      </c>
-      <c r="L68" s="1">
-        <v>518000000000</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
@@ -3098,7 +3089,7 @@
         <v>0.2</v>
       </c>
       <c r="D69">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -3113,16 +3104,16 @@
         <v>4078000000000</v>
       </c>
       <c r="I69">
+        <v>571346000000</v>
+      </c>
+      <c r="J69" s="1">
+        <v>74500000000</v>
+      </c>
+      <c r="K69" s="1">
+        <v>517000000000</v>
+      </c>
+      <c r="L69">
         <v>1944000000000</v>
-      </c>
-      <c r="J69">
-        <v>571346000000</v>
-      </c>
-      <c r="K69" s="1">
-        <v>74500000000</v>
-      </c>
-      <c r="L69" s="1">
-        <v>517000000000</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
@@ -3136,7 +3127,7 @@
         <v>0.2</v>
       </c>
       <c r="D70">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -3151,16 +3142,16 @@
         <v>4092000000000</v>
       </c>
       <c r="I70">
+        <v>539311000000</v>
+      </c>
+      <c r="J70" s="1">
+        <v>74000000000</v>
+      </c>
+      <c r="K70" s="1">
+        <v>499000000000</v>
+      </c>
+      <c r="L70">
         <v>1916000000000</v>
-      </c>
-      <c r="J70">
-        <v>539311000000</v>
-      </c>
-      <c r="K70" s="1">
-        <v>74000000000</v>
-      </c>
-      <c r="L70" s="1">
-        <v>499000000000</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
@@ -3174,7 +3165,7 @@
         <v>0.2</v>
       </c>
       <c r="D71">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -3189,16 +3180,16 @@
         <v>4106000000000</v>
       </c>
       <c r="I71">
+        <v>518566000000</v>
+      </c>
+      <c r="J71" s="1">
+        <v>73300000000</v>
+      </c>
+      <c r="K71" s="1">
+        <v>495000000000</v>
+      </c>
+      <c r="L71">
         <v>1888000000000</v>
-      </c>
-      <c r="J71">
-        <v>518566000000</v>
-      </c>
-      <c r="K71" s="1">
-        <v>73300000000</v>
-      </c>
-      <c r="L71" s="1">
-        <v>495000000000</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
@@ -3212,7 +3203,7 @@
         <v>0.2</v>
       </c>
       <c r="D72">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -3227,16 +3218,16 @@
         <v>4120000000000</v>
       </c>
       <c r="I72">
+        <v>539746000000</v>
+      </c>
+      <c r="J72" s="1">
+        <v>72800000000</v>
+      </c>
+      <c r="K72" s="1">
+        <v>491000000000</v>
+      </c>
+      <c r="L72">
         <v>1860000000000</v>
-      </c>
-      <c r="J72">
-        <v>539746000000</v>
-      </c>
-      <c r="K72" s="1">
-        <v>72800000000</v>
-      </c>
-      <c r="L72" s="1">
-        <v>491000000000</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
@@ -3250,7 +3241,7 @@
         <v>0.2</v>
       </c>
       <c r="D73">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -3265,16 +3256,16 @@
         <v>4130000000000</v>
       </c>
       <c r="I73">
+        <v>610235000000</v>
+      </c>
+      <c r="J73" s="1">
+        <v>69600000000</v>
+      </c>
+      <c r="K73" s="1">
+        <v>470000000000</v>
+      </c>
+      <c r="L73">
         <v>1838000000000</v>
-      </c>
-      <c r="J73">
-        <v>610235000000</v>
-      </c>
-      <c r="K73" s="1">
-        <v>69600000000</v>
-      </c>
-      <c r="L73" s="1">
-        <v>470000000000</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
@@ -3288,7 +3279,7 @@
         <v>0.2</v>
       </c>
       <c r="D74">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E74">
         <v>1</v>
@@ -3303,16 +3294,16 @@
         <v>4140000000000</v>
       </c>
       <c r="I74">
+        <v>587095000000</v>
+      </c>
+      <c r="J74" s="1">
+        <v>69900000000</v>
+      </c>
+      <c r="K74" s="1">
+        <v>459000000000</v>
+      </c>
+      <c r="L74">
         <v>1816000000000</v>
-      </c>
-      <c r="J74">
-        <v>587095000000</v>
-      </c>
-      <c r="K74" s="1">
-        <v>69900000000</v>
-      </c>
-      <c r="L74" s="1">
-        <v>459000000000</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
@@ -3326,7 +3317,7 @@
         <v>0.2</v>
       </c>
       <c r="D75">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -3341,16 +3332,16 @@
         <v>4150000000000</v>
       </c>
       <c r="I75">
+        <v>546138000000</v>
+      </c>
+      <c r="J75" s="1">
+        <v>69400000000</v>
+      </c>
+      <c r="K75" s="1">
+        <v>454000000000</v>
+      </c>
+      <c r="L75">
         <v>1794000000000</v>
-      </c>
-      <c r="J75">
-        <v>546138000000</v>
-      </c>
-      <c r="K75" s="1">
-        <v>69400000000</v>
-      </c>
-      <c r="L75" s="1">
-        <v>454000000000</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
@@ -3364,7 +3355,7 @@
         <v>0.2</v>
       </c>
       <c r="D76">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -3379,16 +3370,16 @@
         <v>4160000000000</v>
       </c>
       <c r="I76">
+        <v>549535000000</v>
+      </c>
+      <c r="J76" s="1">
+        <v>71600000000</v>
+      </c>
+      <c r="K76" s="1">
+        <v>447000000000</v>
+      </c>
+      <c r="L76">
         <v>1772000000000</v>
-      </c>
-      <c r="J76">
-        <v>549535000000</v>
-      </c>
-      <c r="K76" s="1">
-        <v>71600000000</v>
-      </c>
-      <c r="L76" s="1">
-        <v>447000000000</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
@@ -3402,7 +3393,7 @@
         <v>0.2</v>
       </c>
       <c r="D77">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -3417,16 +3408,16 @@
         <v>4170000000000</v>
       </c>
       <c r="I77">
+        <v>638143000000</v>
+      </c>
+      <c r="J77" s="1">
+        <v>68100000000</v>
+      </c>
+      <c r="K77" s="1">
+        <v>441000000000</v>
+      </c>
+      <c r="L77">
         <v>1750000000000</v>
-      </c>
-      <c r="J77">
-        <v>638143000000</v>
-      </c>
-      <c r="K77" s="1">
-        <v>68100000000</v>
-      </c>
-      <c r="L77" s="1">
-        <v>441000000000</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
@@ -3440,7 +3431,7 @@
         <v>0.2</v>
       </c>
       <c r="D78">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E78">
         <v>1</v>
@@ -3455,16 +3446,16 @@
         <v>4180000000000</v>
       </c>
       <c r="I78">
+        <v>661034000000</v>
+      </c>
+      <c r="J78" s="1">
+        <v>68100000000</v>
+      </c>
+      <c r="K78" s="1">
+        <v>433000000000</v>
+      </c>
+      <c r="L78">
         <v>1734000000000</v>
-      </c>
-      <c r="J78">
-        <v>661034000000</v>
-      </c>
-      <c r="K78" s="1">
-        <v>68100000000</v>
-      </c>
-      <c r="L78" s="1">
-        <v>433000000000</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
@@ -3478,7 +3469,7 @@
         <v>0.2</v>
       </c>
       <c r="D79">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -3493,16 +3484,16 @@
         <v>4190000000000</v>
       </c>
       <c r="I79">
+        <v>590304000000</v>
+      </c>
+      <c r="J79" s="1">
+        <v>67400000000</v>
+      </c>
+      <c r="K79" s="1">
+        <v>424000000000</v>
+      </c>
+      <c r="L79">
         <v>1718000000000</v>
-      </c>
-      <c r="J79">
-        <v>590304000000</v>
-      </c>
-      <c r="K79" s="1">
-        <v>67400000000</v>
-      </c>
-      <c r="L79" s="1">
-        <v>424000000000</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
@@ -3516,7 +3507,7 @@
         <v>0.2</v>
       </c>
       <c r="D80">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -3531,16 +3522,16 @@
         <v>4200000000000</v>
       </c>
       <c r="I80">
+        <v>548224000000</v>
+      </c>
+      <c r="J80" s="1">
+        <v>64900000000</v>
+      </c>
+      <c r="K80" s="1">
+        <v>415000000000</v>
+      </c>
+      <c r="L80">
         <v>1702000000000</v>
-      </c>
-      <c r="J80">
-        <v>548224000000</v>
-      </c>
-      <c r="K80" s="1">
-        <v>64900000000</v>
-      </c>
-      <c r="L80" s="1">
-        <v>415000000000</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
@@ -3554,7 +3545,7 @@
         <v>0.2</v>
       </c>
       <c r="D81">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -3569,16 +3560,16 @@
         <v>4210000000000</v>
       </c>
       <c r="I81">
+        <v>543938000000</v>
+      </c>
+      <c r="J81" s="1">
+        <v>64700000000</v>
+      </c>
+      <c r="K81" s="1">
+        <v>404000000000</v>
+      </c>
+      <c r="L81">
         <v>1686000000000</v>
-      </c>
-      <c r="J81">
-        <v>543938000000</v>
-      </c>
-      <c r="K81" s="1">
-        <v>64700000000</v>
-      </c>
-      <c r="L81" s="1">
-        <v>404000000000</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
@@ -3592,7 +3583,7 @@
         <v>0.2</v>
       </c>
       <c r="D82">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -3607,16 +3598,16 @@
         <v>4220000000000</v>
       </c>
       <c r="I82">
+        <v>560524000000</v>
+      </c>
+      <c r="J82" s="1">
+        <v>62200000000</v>
+      </c>
+      <c r="K82" s="1">
+        <v>395000000000</v>
+      </c>
+      <c r="L82">
         <v>1670000000000</v>
-      </c>
-      <c r="J82">
-        <v>560524000000</v>
-      </c>
-      <c r="K82" s="1">
-        <v>62200000000</v>
-      </c>
-      <c r="L82" s="1">
-        <v>395000000000</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
@@ -3630,7 +3621,7 @@
         <v>0.2</v>
       </c>
       <c r="D83">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -3645,16 +3636,16 @@
         <v>4228000000000</v>
       </c>
       <c r="I83">
+        <v>559543000000</v>
+      </c>
+      <c r="J83" s="1">
+        <v>63200000000</v>
+      </c>
+      <c r="K83" s="1">
+        <v>391000000000</v>
+      </c>
+      <c r="L83">
         <v>1656000000000</v>
-      </c>
-      <c r="J83">
-        <v>559543000000</v>
-      </c>
-      <c r="K83" s="1">
-        <v>63200000000</v>
-      </c>
-      <c r="L83" s="1">
-        <v>391000000000</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
@@ -3668,7 +3659,7 @@
         <v>0.2</v>
       </c>
       <c r="D84">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -3683,16 +3674,16 @@
         <v>4236000000000</v>
       </c>
       <c r="I84">
+        <v>546862000000</v>
+      </c>
+      <c r="J84" s="1">
+        <v>62000000000</v>
+      </c>
+      <c r="K84" s="1">
+        <v>388000000000</v>
+      </c>
+      <c r="L84">
         <v>1642000000000</v>
-      </c>
-      <c r="J84">
-        <v>546862000000</v>
-      </c>
-      <c r="K84" s="1">
-        <v>62000000000</v>
-      </c>
-      <c r="L84" s="1">
-        <v>388000000000</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.2">
@@ -3706,7 +3697,7 @@
         <v>0.2</v>
       </c>
       <c r="D85">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E85">
         <v>1</v>
@@ -3721,16 +3712,16 @@
         <v>4244000000000</v>
       </c>
       <c r="I85">
+        <v>534270000000</v>
+      </c>
+      <c r="J85" s="1">
+        <v>62000000000</v>
+      </c>
+      <c r="K85" s="1">
+        <v>384000000000</v>
+      </c>
+      <c r="L85">
         <v>1628000000000</v>
-      </c>
-      <c r="J85">
-        <v>534270000000</v>
-      </c>
-      <c r="K85" s="1">
-        <v>62000000000</v>
-      </c>
-      <c r="L85" s="1">
-        <v>384000000000</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
@@ -3744,7 +3735,7 @@
         <v>0.2</v>
       </c>
       <c r="D86">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -3759,16 +3750,16 @@
         <v>4252000000000</v>
       </c>
       <c r="I86">
+        <v>556371000000</v>
+      </c>
+      <c r="J86" s="1">
+        <v>59500000000</v>
+      </c>
+      <c r="K86" s="1">
+        <v>377000000000</v>
+      </c>
+      <c r="L86">
         <v>1614000000000</v>
-      </c>
-      <c r="J86">
-        <v>556371000000</v>
-      </c>
-      <c r="K86" s="1">
-        <v>59500000000</v>
-      </c>
-      <c r="L86" s="1">
-        <v>377000000000</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.2">
@@ -3782,7 +3773,7 @@
         <v>0.2</v>
       </c>
       <c r="D87">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -3797,16 +3788,16 @@
         <v>4260000000000</v>
       </c>
       <c r="I87">
+        <v>606189000000</v>
+      </c>
+      <c r="J87" s="1">
+        <v>57600000000</v>
+      </c>
+      <c r="K87" s="1">
+        <v>373000000000</v>
+      </c>
+      <c r="L87">
         <v>1600000000000</v>
-      </c>
-      <c r="J87">
-        <v>606189000000</v>
-      </c>
-      <c r="K87" s="1">
-        <v>57600000000</v>
-      </c>
-      <c r="L87" s="1">
-        <v>373000000000</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.2">
@@ -3820,7 +3811,7 @@
         <v>0.2</v>
       </c>
       <c r="D88">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -3835,16 +3826,16 @@
         <v>4250000000000</v>
       </c>
       <c r="I88">
+        <v>612390000000</v>
+      </c>
+      <c r="J88" s="1">
+        <v>57800000000</v>
+      </c>
+      <c r="K88" s="1">
+        <v>371000000000</v>
+      </c>
+      <c r="L88">
         <v>1580000000000</v>
-      </c>
-      <c r="J88">
-        <v>612390000000</v>
-      </c>
-      <c r="K88" s="1">
-        <v>57800000000</v>
-      </c>
-      <c r="L88" s="1">
-        <v>371000000000</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.2">
@@ -3858,7 +3849,7 @@
         <v>0.2</v>
       </c>
       <c r="D89">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -3873,16 +3864,16 @@
         <v>4240000000000</v>
       </c>
       <c r="I89">
+        <v>635276000000</v>
+      </c>
+      <c r="J89" s="1">
+        <v>56800000000</v>
+      </c>
+      <c r="K89" s="1">
+        <v>369000000000</v>
+      </c>
+      <c r="L89">
         <v>1560000000000</v>
-      </c>
-      <c r="J89">
-        <v>635276000000</v>
-      </c>
-      <c r="K89" s="1">
-        <v>56800000000</v>
-      </c>
-      <c r="L89" s="1">
-        <v>369000000000</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
@@ -3896,7 +3887,7 @@
         <v>0.2</v>
       </c>
       <c r="D90">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E90">
         <v>1</v>
@@ -3911,16 +3902,16 @@
         <v>4230000000000</v>
       </c>
       <c r="I90">
+        <v>629627000000</v>
+      </c>
+      <c r="J90" s="1">
+        <v>56100000000</v>
+      </c>
+      <c r="K90" s="1">
+        <v>361000000000</v>
+      </c>
+      <c r="L90">
         <v>1540000000000</v>
-      </c>
-      <c r="J90">
-        <v>629627000000</v>
-      </c>
-      <c r="K90" s="1">
-        <v>56100000000</v>
-      </c>
-      <c r="L90" s="1">
-        <v>361000000000</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.2">
@@ -3934,7 +3925,7 @@
         <v>0.2</v>
       </c>
       <c r="D91">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E91">
         <v>1</v>
@@ -3949,16 +3940,16 @@
         <v>4220000000000</v>
       </c>
       <c r="I91">
+        <v>590209000000</v>
+      </c>
+      <c r="J91" s="1">
+        <v>55400000000</v>
+      </c>
+      <c r="K91" s="1">
+        <v>355000000000</v>
+      </c>
+      <c r="L91">
         <v>1520000000000</v>
-      </c>
-      <c r="J91">
-        <v>590209000000</v>
-      </c>
-      <c r="K91" s="1">
-        <v>55400000000</v>
-      </c>
-      <c r="L91" s="1">
-        <v>355000000000</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.2">
@@ -3972,7 +3963,7 @@
         <v>0.2</v>
       </c>
       <c r="D92">
-        <v>1013.25</v>
+        <v>101325</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -3987,16 +3978,16 @@
         <v>4210000000000</v>
       </c>
       <c r="I92">
+        <v>571039000000</v>
+      </c>
+      <c r="J92" s="1">
+        <v>55100000000</v>
+      </c>
+      <c r="K92" s="1">
+        <v>352000000000</v>
+      </c>
+      <c r="L92">
         <v>1500000000000</v>
-      </c>
-      <c r="J92">
-        <v>571039000000</v>
-      </c>
-      <c r="K92" s="1">
-        <v>55100000000</v>
-      </c>
-      <c r="L92" s="1">
-        <v>352000000000</v>
       </c>
     </row>
   </sheetData>
@@ -4006,1025 +3997,567 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60206BB5-63D0-9943-A8E8-21A9E6C0DBE3}">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B2:B11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>23777.923999999999</v>
-      </c>
-      <c r="B2" s="2">
-        <v>4.7343389929677397E-2</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>1507786.8525</v>
-      </c>
-      <c r="B3" s="2">
-        <v>4.5863043871237498E-2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>2991795.781</v>
-      </c>
-      <c r="B4" s="2">
-        <v>4.4382697812797599E-2</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>4475804.7094999999</v>
-      </c>
-      <c r="B5" s="2">
-        <v>4.29023517543577E-2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>5959813.6380000003</v>
-      </c>
-      <c r="B6" s="2">
-        <v>4.14220056959178E-2</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>6087737.8854</v>
-      </c>
-      <c r="B7" s="2">
-        <v>4.3914686912226997E-2</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>6215662.1327999998</v>
-      </c>
-      <c r="B8" s="2">
-        <v>4.64073681285362E-2</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>6343586.3801999995</v>
-      </c>
-      <c r="B9" s="2">
-        <v>4.89000493448455E-2</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>6471510.6276000002</v>
-      </c>
-      <c r="B10" s="2">
-        <v>5.1392730561154697E-2</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>6599434.875</v>
-      </c>
-      <c r="B11" s="2">
-        <v>5.38854117774639E-2</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>6566726.4847499998</v>
-      </c>
-      <c r="B12" s="2">
-        <v>5.6007884575260999E-2</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>6534018.0944999997</v>
-      </c>
-      <c r="B13" s="2">
-        <v>5.8130357373058002E-2</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>6501309.7042500004</v>
-      </c>
-      <c r="B14" s="2">
-        <v>6.0252830170854997E-2</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>6468601.3140000002</v>
-      </c>
-      <c r="B15" s="2">
-        <v>6.2375302968652097E-2</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>6396269.1092499997</v>
-      </c>
-      <c r="B16" s="2">
-        <v>6.4054915142224306E-2</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>6323936.9045000002</v>
-      </c>
-      <c r="B17" s="2">
-        <v>6.5734527315796501E-2</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>6251604.6997499997</v>
-      </c>
-      <c r="B18" s="2">
-        <v>6.7414139489368793E-2</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>6179272.4950000001</v>
-      </c>
-      <c r="B19" s="2">
-        <v>6.9093751662941003E-2</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>6113684.9902499998</v>
-      </c>
-      <c r="B20" s="2">
-        <v>7.0348060082381203E-2</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>6048097.4855000004</v>
-      </c>
-      <c r="B21" s="2">
-        <v>7.1602368501821403E-2</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>5982509.9807500001</v>
-      </c>
-      <c r="B22" s="2">
-        <v>7.2856676921261507E-2</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>5916922.4759999998</v>
-      </c>
-      <c r="B23" s="2">
-        <v>7.4110985340701693E-2</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
-        <v>5861611.6431999998</v>
-      </c>
-      <c r="B24" s="2">
-        <v>7.4967808360838398E-2</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>5806300.8103999998</v>
-      </c>
-      <c r="B25" s="2">
-        <v>7.5824631380975005E-2</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <v>5750989.9775999999</v>
-      </c>
-      <c r="B26" s="2">
-        <v>7.6681454401111696E-2</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
-        <v>5695679.1447999999</v>
-      </c>
-      <c r="B27" s="2">
-        <v>7.7538277421248303E-2</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
-        <v>5640368.3119999999</v>
-      </c>
-      <c r="B28" s="2">
-        <v>7.8395100441384993E-2</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>5579380.7402499998</v>
-      </c>
-      <c r="B29" s="2">
-        <v>7.92777747228747E-2</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>5518393.1684999997</v>
-      </c>
-      <c r="B30" s="2">
-        <v>8.0160449004364503E-2</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
-        <v>5457405.5967499996</v>
-      </c>
-      <c r="B31" s="2">
-        <v>8.1043123285854293E-2</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
-        <v>5396418.0250000004</v>
-      </c>
-      <c r="B32" s="2">
-        <v>8.1925797567344097E-2</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
-        <v>5346145.1992499996</v>
-      </c>
-      <c r="B33" s="2">
-        <v>8.2640995551758994E-2</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
-        <v>5295872.3734999998</v>
-      </c>
-      <c r="B34" s="2">
-        <v>8.3356193536173906E-2</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
-        <v>5245599.5477499999</v>
-      </c>
-      <c r="B35" s="2">
-        <v>8.4071391520588803E-2</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
-        <v>5195326.7220000001</v>
-      </c>
-      <c r="B36" s="2">
-        <v>8.4786589505003798E-2</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
-        <v>5160085.8952500001</v>
-      </c>
-      <c r="B37" s="2">
-        <v>8.5510990223238895E-2</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
-        <v>5124845.0685000001</v>
-      </c>
-      <c r="B38" s="2">
-        <v>8.6235390941474005E-2</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
-        <v>5089604.24175</v>
-      </c>
-      <c r="B39" s="2">
-        <v>8.6959791659709101E-2</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
-        <v>5016511.7737999996</v>
-      </c>
-      <c r="B40" s="2">
-        <v>8.8169824721344006E-2</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
-        <v>4978660.1326000001</v>
-      </c>
-      <c r="B41" s="2">
-        <v>8.8655457064743898E-2</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
-        <v>4940808.4913999997</v>
-      </c>
-      <c r="B42" s="2">
-        <v>8.9141089408143803E-2</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
-        <v>4902956.8502000002</v>
-      </c>
-      <c r="B43" s="2">
-        <v>8.9626721751543695E-2</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
-        <v>4865105.2089999998</v>
-      </c>
-      <c r="B44" s="2">
-        <v>9.0112354094943503E-2</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
-        <v>4841576.3922499996</v>
-      </c>
-      <c r="B45" s="2">
-        <v>9.0637694112668296E-2</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
-        <v>4818047.5755000003</v>
-      </c>
-      <c r="B46" s="2">
-        <v>9.1163034130393006E-2</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
-        <v>4794518.75875</v>
-      </c>
-      <c r="B47" s="2">
-        <v>9.1688374148117799E-2</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
-        <v>4770989.9419999998</v>
-      </c>
-      <c r="B48" s="2">
-        <v>9.2213714165842495E-2</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="2">
-        <v>4730225.0690000001</v>
-      </c>
-      <c r="B49" s="2">
-        <v>9.2708231606264499E-2</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
-        <v>4689460.1960000005</v>
-      </c>
-      <c r="B50" s="2">
-        <v>9.3202749046686503E-2</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="2">
-        <v>4648695.3229999999</v>
-      </c>
-      <c r="B51" s="2">
-        <v>9.3697266487108494E-2</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="2">
-        <v>4607930.45</v>
-      </c>
-      <c r="B52" s="2">
-        <v>9.4191783927530498E-2</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="2">
-        <v>4566436.0554999998</v>
-      </c>
-      <c r="B53" s="2">
-        <v>9.4562403399412895E-2</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="2">
-        <v>4524941.6610000003</v>
-      </c>
-      <c r="B54" s="2">
-        <v>9.4933022871295403E-2</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="2">
-        <v>4483447.2664999999</v>
-      </c>
-      <c r="B55" s="2">
-        <v>9.5303642343177897E-2</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="2">
-        <v>4441952.8720000004</v>
-      </c>
-      <c r="B56" s="2">
-        <v>9.5674261815060405E-2</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="2">
-        <v>4419514.0549999997</v>
-      </c>
-      <c r="B57" s="2">
-        <v>9.5971667134555405E-2</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="2">
-        <v>4397075.2379999999</v>
-      </c>
-      <c r="B58" s="2">
-        <v>9.6269072454050503E-2</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="2">
-        <v>4374636.4210000001</v>
-      </c>
-      <c r="B59" s="2">
-        <v>9.65664777735456E-2</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="2">
-        <v>4352197.60399999</v>
-      </c>
-      <c r="B60" s="2">
-        <v>9.6863883093040698E-2</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="2">
-        <v>4329758.7869999995</v>
-      </c>
-      <c r="B61" s="2">
-        <v>9.7161288412535796E-2</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="2">
-        <v>4300713.085</v>
-      </c>
-      <c r="B62" s="2">
-        <v>9.7564002689682905E-2</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="2">
-        <v>4271667.3829999901</v>
-      </c>
-      <c r="B63" s="2">
-        <v>9.7966716966830097E-2</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="2">
-        <v>4242621.6809999999</v>
-      </c>
-      <c r="B64" s="2">
-        <v>9.8369431243977304E-2</v>
-      </c>
-      <c r="C64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="2">
-        <v>4213575.9790000003</v>
-      </c>
-      <c r="B65" s="2">
-        <v>9.8772145521124399E-2</v>
-      </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="2">
-        <v>4195691.8344999999</v>
-      </c>
-      <c r="B66" s="2">
-        <v>9.9144973278636403E-2</v>
-      </c>
-      <c r="C66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="2">
-        <v>4177807.69</v>
-      </c>
-      <c r="B67" s="2">
-        <v>9.9517801036148407E-2</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="2">
-        <v>4159923.5455</v>
-      </c>
-      <c r="B68" s="2">
-        <v>9.9890628793660396E-2</v>
-      </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="2">
-        <v>4142039.4010000001</v>
-      </c>
-      <c r="B69" s="2">
-        <v>0.100263456551172</v>
-      </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="2">
-        <v>4126212.1165999998</v>
-      </c>
-      <c r="B70" s="2">
-        <v>0.10049115957371101</v>
-      </c>
-      <c r="C70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="2">
-        <v>4110384.8322000001</v>
-      </c>
-      <c r="B71" s="2">
-        <v>0.100718862596251</v>
-      </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="2">
-        <v>4094557.5477999998</v>
-      </c>
-      <c r="B72" s="2">
-        <v>0.10094656561878999</v>
-      </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="2">
-        <v>4078730.2634000001</v>
-      </c>
-      <c r="B73" s="2">
-        <v>0.10117426864133</v>
-      </c>
-      <c r="C73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="2">
-        <v>4062902.9789999998</v>
-      </c>
-      <c r="B74" s="2">
-        <v>0.10140197166386899</v>
-      </c>
-      <c r="C74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="2">
-        <v>4043553.6954999999</v>
-      </c>
-      <c r="B75" s="2">
-        <v>0.101637682073348</v>
-      </c>
-      <c r="C75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="2">
-        <v>4024204.412</v>
-      </c>
-      <c r="B76" s="2">
-        <v>0.10187339248282699</v>
-      </c>
-      <c r="C76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="2">
-        <v>4004855.1285000001</v>
-      </c>
-      <c r="B77" s="2">
-        <v>0.102109102892305</v>
-      </c>
-      <c r="C77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="2">
-        <v>3985505.8450000002</v>
-      </c>
-      <c r="B78" s="2">
-        <v>0.10234481330178399</v>
-      </c>
-      <c r="C78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="2">
-        <v>3960595.2722499999</v>
-      </c>
-      <c r="B79" s="2">
-        <v>0.102627607685742</v>
-      </c>
-      <c r="C79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="2">
-        <v>3935684.6995000001</v>
-      </c>
-      <c r="B80" s="2">
-        <v>0.10291040206969999</v>
-      </c>
-      <c r="C80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="2">
-        <v>3910774.1267499998</v>
-      </c>
-      <c r="B81" s="2">
-        <v>0.103193196453657</v>
-      </c>
-      <c r="C81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="2">
-        <v>3885863.554</v>
-      </c>
-      <c r="B82" s="2">
-        <v>0.103475990837615</v>
-      </c>
-      <c r="C82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="2">
-        <v>3853813.8295</v>
-      </c>
-      <c r="B83" s="2">
-        <v>0.103726318770455</v>
-      </c>
-      <c r="C83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="2">
-        <v>3821764.105</v>
-      </c>
-      <c r="B84" s="2">
-        <v>0.103976646703296</v>
-      </c>
-      <c r="C84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="2">
-        <v>3789714.3805</v>
-      </c>
-      <c r="B85" s="2">
-        <v>0.104226974636136</v>
-      </c>
-      <c r="C85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="2">
-        <v>3757664.656</v>
-      </c>
-      <c r="B86" s="2">
-        <v>0.104477302568976</v>
-      </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="2">
-        <v>3757664.656</v>
-      </c>
-      <c r="B87" s="2">
-        <v>0.104477302568976</v>
-      </c>
-      <c r="C87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="2">
-        <v>3757664.656</v>
-      </c>
-      <c r="B88" s="2">
-        <v>0.104477302568976</v>
-      </c>
-      <c r="C88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="2">
-        <v>3757664.656</v>
-      </c>
-      <c r="B89" s="2">
-        <v>0.104477302568976</v>
-      </c>
-      <c r="C89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="2">
-        <v>3757664.656</v>
-      </c>
-      <c r="B90" s="2">
-        <v>0.104477302568976</v>
-      </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="2">
-        <v>3757664.656</v>
-      </c>
-      <c r="B91" s="2">
-        <v>0.104477302568976</v>
-      </c>
-      <c r="C91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="2">
-        <v>3757664.656</v>
-      </c>
-      <c r="B92" s="2">
-        <v>0.104477302568976</v>
-      </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>10900000000000</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10574000000000</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>10248000000000</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>9922000000000</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>9596000000000</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>9270000000000</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>9016000000000</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8762000000000</v>
+      </c>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8508000000000</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8254000000000</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8000000000000</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>7774000000000</v>
+      </c>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>7548000000000</v>
+      </c>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>7322000000000</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>7096000000000</v>
+      </c>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>6870000000000</v>
+      </c>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>6670000000000</v>
+      </c>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>6470000000000</v>
+      </c>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>6270000000000</v>
+      </c>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>6070000000000</v>
+      </c>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>5870000000000</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>5696000000000</v>
+      </c>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>5522000000000</v>
+      </c>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>5348000000000</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>5174000000000</v>
+      </c>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>5000000000000</v>
+      </c>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>4872000000000</v>
+      </c>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>4744000000000</v>
+      </c>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>4616000000000</v>
+      </c>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>4488000000000</v>
+      </c>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>4360000000000</v>
+      </c>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>4256000000000</v>
+      </c>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>4152000000000</v>
+      </c>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>4048000000000</v>
+      </c>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3944000000000</v>
+      </c>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>3840000000000</v>
+      </c>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>3750000000000</v>
+      </c>
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3660000000000</v>
+      </c>
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3480000000000</v>
+      </c>
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>3390000000000</v>
+      </c>
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>3314000000000</v>
+      </c>
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>3238000000000</v>
+      </c>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>3162000000000</v>
+      </c>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>3086000000000</v>
+      </c>
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>3010000000000</v>
+      </c>
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2956666666666.6602</v>
+      </c>
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2903333333333.3301</v>
+      </c>
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2850000000000</v>
+      </c>
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2796666666666.6602</v>
+      </c>
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2743333333333.3301</v>
+      </c>
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2690000000000</v>
+      </c>
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2640000000000</v>
+      </c>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>2590000000000</v>
+      </c>
+      <c r="B54" s="2"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>2540000000000</v>
+      </c>
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>2490000000000</v>
+      </c>
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>2440000000000</v>
+      </c>
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2396000000000</v>
+      </c>
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>2352000000000</v>
+      </c>
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>2308000000000</v>
+      </c>
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>2264000000000</v>
+      </c>
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>2220000000000</v>
+      </c>
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2176000000000</v>
+      </c>
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>2132000000000</v>
+      </c>
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>2088000000000</v>
+      </c>
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>2044000000000</v>
+      </c>
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>2000000000000</v>
+      </c>
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>1972000000000</v>
+      </c>
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>1944000000000</v>
+      </c>
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>1916000000000</v>
+      </c>
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>1888000000000</v>
+      </c>
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>1860000000000</v>
+      </c>
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>1838000000000</v>
+      </c>
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>1816000000000</v>
+      </c>
+      <c r="B74" s="2"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>1794000000000</v>
+      </c>
+      <c r="B75" s="2"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>1772000000000</v>
+      </c>
+      <c r="B76" s="2"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>1750000000000</v>
+      </c>
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>1734000000000</v>
+      </c>
+      <c r="B78" s="2"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>1718000000000</v>
+      </c>
+      <c r="B79" s="2"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>1702000000000</v>
+      </c>
+      <c r="B80" s="2"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>1686000000000</v>
+      </c>
+      <c r="B81" s="2"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>1670000000000</v>
+      </c>
+      <c r="B82" s="2"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>1656000000000</v>
+      </c>
+      <c r="B83" s="2"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>1642000000000</v>
+      </c>
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>1628000000000</v>
+      </c>
+      <c r="B85" s="2"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>1614000000000</v>
+      </c>
+      <c r="B86" s="2"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>1600000000000</v>
+      </c>
+      <c r="B87" s="2"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>1580000000000</v>
+      </c>
+      <c r="B88" s="2"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>1560000000000</v>
+      </c>
+      <c r="B89" s="2"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>1540000000000</v>
+      </c>
+      <c r="B90" s="2"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>1520000000000</v>
+      </c>
+      <c r="B91" s="2"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>1500000000000</v>
+      </c>
+      <c r="B92" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>